<commit_message>
Added parts for display
</commit_message>
<xml_diff>
--- a/Research/Major Parts.xlsx
+++ b/Research/Major Parts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEFF00D-4CD6-4E2E-8A24-EC9A254C770B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7925E38-30E2-460B-B60A-090A3B042818}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Main AC/DC converter </t>
   </si>
@@ -47,6 +47,42 @@
   </si>
   <si>
     <t>DC/DC 5.0V</t>
+  </si>
+  <si>
+    <t>Display:</t>
+  </si>
+  <si>
+    <t>Multi Meters</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/McIgIcM-Digital-Voltmeter-Ammeter-10ADetector/dp/B06XR2XKNT/ref=sr_1_7?keywords=digital+current+meter&amp;qid=1561517841&amp;s=industrial&amp;sr=1-7</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/705/1528-1149-ND/5353609</t>
+  </si>
+  <si>
+    <t>Volt Meters</t>
+  </si>
+  <si>
+    <t>http://easycircuit012.blogspot.com/2012/12/digital-volt-and-ampere-meter-circuit.html</t>
+  </si>
+  <si>
+    <t>Design it on your own</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lumex-opto-components-inc/LDT-A512RI/67-1424-ND/252626</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lumex-opto-components-inc/LDT-A514RI/67-1423-ND/252628</t>
+  </si>
+  <si>
+    <t>http://www.electronics-diy.com/70v_pic_voltmeter_amperemeter.php</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/399?gclid=Cj0KCQjwjMfoBRDDARIsAMUjNZpkoKOfF8LGOWSxf4VLWIPIVsbuiiDFCeu1C8yUAKVEhcIb9canXt8aAnndEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/PIC16F876A-I%2fSO/PIC16F876A-I%2fSO-ND/446139/?itemSeq=296474682</t>
   </si>
 </sst>
 </file>
@@ -375,13 +411,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A16"/>
+  <dimension ref="A2:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -432,6 +471,60 @@
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -441,6 +534,14 @@
     <hyperlink ref="A10" r:id="rId3" xr:uid="{8402C350-2BF3-4845-BA8C-A1A552DE932C}"/>
     <hyperlink ref="A13" r:id="rId4" xr:uid="{7D6CE2C4-2208-4168-B600-1D7BD9F892DC}"/>
     <hyperlink ref="A16" r:id="rId5" xr:uid="{EC52643B-782E-45F0-873A-57FC803692D6}"/>
+    <hyperlink ref="B21" r:id="rId6" xr:uid="{F9688411-06E8-49EC-B469-7D5B1C57FBA8}"/>
+    <hyperlink ref="B23" r:id="rId7" xr:uid="{7C742F7B-2741-4678-8A53-1D63726F7A8E}"/>
+    <hyperlink ref="B25" r:id="rId8" xr:uid="{2F38268A-E5FA-4597-A8C6-01E62C9D57E1}"/>
+    <hyperlink ref="B27" r:id="rId9" xr:uid="{DAE5B022-B6B9-4B00-B5C4-E6A00A9DFA12}"/>
+    <hyperlink ref="B28" r:id="rId10" xr:uid="{EE6081D1-55ED-4CB9-85BC-82753EED7351}"/>
+    <hyperlink ref="B30" r:id="rId11" xr:uid="{777F2CA4-3CA8-4983-8F72-47073529350C}"/>
+    <hyperlink ref="B31" r:id="rId12" xr:uid="{0172D380-E36C-4D1E-936B-1089917732FA}"/>
+    <hyperlink ref="B32" r:id="rId13" xr:uid="{05C716E0-E13B-4A77-BB47-D48C39AD8D17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished adding all the major parts
</commit_message>
<xml_diff>
--- a/Research/Major Parts.xlsx
+++ b/Research/Major Parts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68E391B-0F81-4EBB-A7C9-54637E96BAAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3229A26-FF9F-40D0-8230-4146F4CAC2F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Main AC/DC converter </t>
   </si>
@@ -86,13 +86,28 @@
   </si>
   <si>
     <t>USB Connectors</t>
+  </si>
+  <si>
+    <t>Binding Posts:</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sparkfun-electronics/PRT-09740/1568-1665-ND/7393681</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sparkfun-electronics/PRT-09739/1568-1664-ND/7393680</t>
+  </si>
+  <si>
+    <t>https://www.ebay.ie/itm/DIY-PCB-Banana-jack-binding-post-breakout-board-/163248841920</t>
+  </si>
+  <si>
+    <t>MAJOR PARTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +126,14 @@
     <font>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,10 +160,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -165,13 +191,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>6376</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9072</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>103645</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -209,14 +235,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>208645</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>63501</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>119012</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>119011</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -253,13 +279,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>308428</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>80059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>3857</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>66142</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -559,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B44"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,126 +596,161 @@
     <col min="1" max="1" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B41" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B42" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B45" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{380C03C9-88AF-4035-B734-60A7F7453C01}"/>
-    <hyperlink ref="A9" r:id="rId2" xr:uid="{4BD1D090-9A86-4DF8-BD8D-0553F60F1558}"/>
-    <hyperlink ref="A32" r:id="rId3" xr:uid="{7D6CE2C4-2208-4168-B600-1D7BD9F892DC}"/>
-    <hyperlink ref="A35" r:id="rId4" xr:uid="{EC52643B-782E-45F0-873A-57FC803692D6}"/>
-    <hyperlink ref="B40" r:id="rId5" xr:uid="{777F2CA4-3CA8-4983-8F72-47073529350C}"/>
-    <hyperlink ref="B41" r:id="rId6" xr:uid="{0172D380-E36C-4D1E-936B-1089917732FA}"/>
-    <hyperlink ref="B42" r:id="rId7" xr:uid="{05C716E0-E13B-4A77-BB47-D48C39AD8D17}"/>
-    <hyperlink ref="A11" r:id="rId8" xr:uid="{697F6185-1489-4B89-879C-C7B622F9805D}"/>
-    <hyperlink ref="B26" r:id="rId9" xr:uid="{20C952C0-AC93-4997-B0E6-DDB49E73E6C8}"/>
-    <hyperlink ref="B27" r:id="rId10" xr:uid="{9ED0288B-B903-4B95-A943-B00D22643BB3}"/>
-    <hyperlink ref="B44" r:id="rId11" xr:uid="{1CBDC011-B012-4D4D-85BE-815CAF394EF8}"/>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{380C03C9-88AF-4035-B734-60A7F7453C01}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{4BD1D090-9A86-4DF8-BD8D-0553F60F1558}"/>
+    <hyperlink ref="A36" r:id="rId3" xr:uid="{7D6CE2C4-2208-4168-B600-1D7BD9F892DC}"/>
+    <hyperlink ref="A39" r:id="rId4" xr:uid="{EC52643B-782E-45F0-873A-57FC803692D6}"/>
+    <hyperlink ref="B44" r:id="rId5" xr:uid="{777F2CA4-3CA8-4983-8F72-47073529350C}"/>
+    <hyperlink ref="B45" r:id="rId6" xr:uid="{0172D380-E36C-4D1E-936B-1089917732FA}"/>
+    <hyperlink ref="B46" r:id="rId7" xr:uid="{05C716E0-E13B-4A77-BB47-D48C39AD8D17}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{697F6185-1489-4B89-879C-C7B622F9805D}"/>
+    <hyperlink ref="B30" r:id="rId9" xr:uid="{20C952C0-AC93-4997-B0E6-DDB49E73E6C8}"/>
+    <hyperlink ref="B31" r:id="rId10" xr:uid="{9ED0288B-B903-4B95-A943-B00D22643BB3}"/>
+    <hyperlink ref="B48" r:id="rId11" xr:uid="{1CBDC011-B012-4D4D-85BE-815CAF394EF8}"/>
+    <hyperlink ref="B50" r:id="rId12" xr:uid="{933C97F6-B8AD-43AB-BDA5-8CE80E8B0DE0}"/>
+    <hyperlink ref="B51" r:id="rId13" xr:uid="{F9022034-5431-4C29-9A17-2E7AA4504D96}"/>
+    <hyperlink ref="B53" r:id="rId14" xr:uid="{68F48E87-03C9-4A06-9ABC-AD2472F277D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId12"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added PIC microcontroller simulation and firmware
</commit_message>
<xml_diff>
--- a/Research/Major Parts.xlsx
+++ b/Research/Major Parts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F773C723-9913-4A87-9848-EE4E68526A24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3932DC0-FB7B-47AB-B281-F85B4111216B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added ADC simulation/code for Current/Voltage measurements
</commit_message>
<xml_diff>
--- a/Research/Major Parts.xlsx
+++ b/Research/Major Parts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3932DC0-FB7B-47AB-B281-F85B4111216B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6AB57D-9F6B-4773-A791-46560E553656}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Main AC/DC converter </t>
   </si>
@@ -55,12 +55,6 @@
     <t>https://www.adafruit.com/product/399?gclid=Cj0KCQjwjMfoBRDDARIsAMUjNZpkoKOfF8LGOWSxf4VLWIPIVsbuiiDFCeu1C8yUAKVEhcIb9canXt8aAnndEALw_wcB</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/PIC16F876A-I%2fSO/PIC16F876A-I%2fSO-ND/446139/?itemSeq=296474682</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/linear-technology-analog-devices/LT3086EFE-TRPBF/LT3086EFE-TRPBFTR-ND/5233238</t>
-  </si>
-  <si>
     <t>Pots for the Buck</t>
   </si>
   <si>
@@ -107,6 +101,24 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/bel-fuse-inc/0685H9250-01/507-1946-2-ND/5466709</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/linear-technology-analog-devices/LT3086EFE-PBF/LT3086EFE-PBF-ND/4755521</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/on-shore-technology-inc/ED281DT/ED3050-5-ND/4147600?cur=CAD&amp;lang=en</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/PIC16F876A-I-SP/PIC16F876A-I-SP-ND/446140?utm_adgroup=Integrated%20Circuits&amp;slid=&amp;gclid=CjwKCAjw6vvoBRBtEiwAZq-T1cbpSSrT8i9aODTro_MTEWrs2Wxml9AlMopeLFXJOV1RSkFyex71UhoCVq4QAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/vishay-dale/RS0101R000FE73/RSD-1.0RTR-ND/1166364</t>
+  </si>
+  <si>
+    <t>Current Limit Set Switch</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/c-k/KS12R22CQD/CKN1595-ND/484129</t>
   </si>
 </sst>
 </file>
@@ -317,6 +329,50 @@
         <a:xfrm>
           <a:off x="5569857" y="2257202"/>
           <a:ext cx="1518786" cy="530369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>172871</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>56371</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF647587-1B9B-4FD3-A871-B7A6D5CEC71F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7207250" y="3066895"/>
+          <a:ext cx="4332121" cy="1923426"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -591,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,7 +660,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -636,7 +692,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -644,23 +700,31 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -703,49 +767,59 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B47" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
       <c r="B48" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>25</v>
-      </c>
       <c r="B55" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -755,18 +829,21 @@
     <hyperlink ref="A39" r:id="rId3" xr:uid="{EC52643B-782E-45F0-873A-57FC803692D6}"/>
     <hyperlink ref="B44" r:id="rId4" xr:uid="{777F2CA4-3CA8-4983-8F72-47073529350C}"/>
     <hyperlink ref="B45" r:id="rId5" xr:uid="{0172D380-E36C-4D1E-936B-1089917732FA}"/>
-    <hyperlink ref="B46" r:id="rId6" xr:uid="{05C716E0-E13B-4A77-BB47-D48C39AD8D17}"/>
-    <hyperlink ref="A13" r:id="rId7" xr:uid="{697F6185-1489-4B89-879C-C7B622F9805D}"/>
-    <hyperlink ref="B30" r:id="rId8" xr:uid="{20C952C0-AC93-4997-B0E6-DDB49E73E6C8}"/>
-    <hyperlink ref="B31" r:id="rId9" xr:uid="{9ED0288B-B903-4B95-A943-B00D22643BB3}"/>
-    <hyperlink ref="B48" r:id="rId10" xr:uid="{1CBDC011-B012-4D4D-85BE-815CAF394EF8}"/>
-    <hyperlink ref="B50" r:id="rId11" xr:uid="{933C97F6-B8AD-43AB-BDA5-8CE80E8B0DE0}"/>
-    <hyperlink ref="B51" r:id="rId12" xr:uid="{F9022034-5431-4C29-9A17-2E7AA4504D96}"/>
-    <hyperlink ref="B53" r:id="rId13" xr:uid="{68F48E87-03C9-4A06-9ABC-AD2472F277D4}"/>
-    <hyperlink ref="B55" r:id="rId14" xr:uid="{4CFE8BA0-D183-4C26-9CA9-BEC5D4FEB2AF}"/>
-    <hyperlink ref="B57" r:id="rId15" xr:uid="{76008964-D3A6-4069-A099-FCBDC9806B52}"/>
+    <hyperlink ref="B30" r:id="rId6" xr:uid="{20C952C0-AC93-4997-B0E6-DDB49E73E6C8}"/>
+    <hyperlink ref="B31" r:id="rId7" xr:uid="{9ED0288B-B903-4B95-A943-B00D22643BB3}"/>
+    <hyperlink ref="B50" r:id="rId8" xr:uid="{1CBDC011-B012-4D4D-85BE-815CAF394EF8}"/>
+    <hyperlink ref="B52" r:id="rId9" xr:uid="{933C97F6-B8AD-43AB-BDA5-8CE80E8B0DE0}"/>
+    <hyperlink ref="B53" r:id="rId10" xr:uid="{F9022034-5431-4C29-9A17-2E7AA4504D96}"/>
+    <hyperlink ref="B55" r:id="rId11" xr:uid="{68F48E87-03C9-4A06-9ABC-AD2472F277D4}"/>
+    <hyperlink ref="B57" r:id="rId12" xr:uid="{4CFE8BA0-D183-4C26-9CA9-BEC5D4FEB2AF}"/>
+    <hyperlink ref="B59" r:id="rId13" xr:uid="{76008964-D3A6-4069-A099-FCBDC9806B52}"/>
+    <hyperlink ref="A13" r:id="rId14" xr:uid="{2D260EA6-B6E3-49E5-AFF7-A6AAA0D9D5F1}"/>
+    <hyperlink ref="B47" r:id="rId15" xr:uid="{BD37EAD5-5C34-4550-93BE-F5FEABEB65A8}"/>
+    <hyperlink ref="B46" r:id="rId16" xr:uid="{4E70A93A-2FD3-4A64-BFD8-40CC5D4AB6CA}"/>
+    <hyperlink ref="B48" r:id="rId17" xr:uid="{FA6B2910-1118-4545-AA35-6807A2305F66}"/>
+    <hyperlink ref="B33" r:id="rId18" xr:uid="{31F1E98B-22F1-4AAD-A4F2-1D4E1C61AC62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Power input schematic page
</commit_message>
<xml_diff>
--- a/Research/Major Parts.xlsx
+++ b/Research/Major Parts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6AB57D-9F6B-4773-A791-46560E553656}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED10CB-BD6E-4ACF-93C4-71B0FA1816D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Main AC/DC converter </t>
   </si>
@@ -52,9 +52,6 @@
     <t>http://www.electronics-diy.com/70v_pic_voltmeter_amperemeter.php</t>
   </si>
   <si>
-    <t>https://www.adafruit.com/product/399?gclid=Cj0KCQjwjMfoBRDDARIsAMUjNZpkoKOfF8LGOWSxf4VLWIPIVsbuiiDFCeu1C8yUAKVEhcIb9canXt8aAnndEALw_wcB</t>
-  </si>
-  <si>
     <t>Pots for the Buck</t>
   </si>
   <si>
@@ -97,12 +94,6 @@
     <t>https://www.digikey.ca/products/en?keywords=KP01.1112.11</t>
   </si>
   <si>
-    <t>AC Fuse</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/bel-fuse-inc/0685H9250-01/507-1946-2-ND/5466709</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/linear-technology-analog-devices/LT3086EFE-PBF/LT3086EFE-PBF-ND/4755521</t>
   </si>
   <si>
@@ -119,6 +110,9 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/c-k/KS12R22CQD/CKN1595-ND/484129</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/adafruit-industries-llc/399/1528-1506-ND/5774232</t>
   </si>
 </sst>
 </file>
@@ -649,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,7 +654,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -692,7 +686,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -700,31 +694,31 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -762,65 +756,60 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B47" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B59" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -828,22 +817,21 @@
     <hyperlink ref="A36" r:id="rId2" xr:uid="{7D6CE2C4-2208-4168-B600-1D7BD9F892DC}"/>
     <hyperlink ref="A39" r:id="rId3" xr:uid="{EC52643B-782E-45F0-873A-57FC803692D6}"/>
     <hyperlink ref="B44" r:id="rId4" xr:uid="{777F2CA4-3CA8-4983-8F72-47073529350C}"/>
-    <hyperlink ref="B45" r:id="rId5" xr:uid="{0172D380-E36C-4D1E-936B-1089917732FA}"/>
-    <hyperlink ref="B30" r:id="rId6" xr:uid="{20C952C0-AC93-4997-B0E6-DDB49E73E6C8}"/>
-    <hyperlink ref="B31" r:id="rId7" xr:uid="{9ED0288B-B903-4B95-A943-B00D22643BB3}"/>
-    <hyperlink ref="B50" r:id="rId8" xr:uid="{1CBDC011-B012-4D4D-85BE-815CAF394EF8}"/>
-    <hyperlink ref="B52" r:id="rId9" xr:uid="{933C97F6-B8AD-43AB-BDA5-8CE80E8B0DE0}"/>
-    <hyperlink ref="B53" r:id="rId10" xr:uid="{F9022034-5431-4C29-9A17-2E7AA4504D96}"/>
-    <hyperlink ref="B55" r:id="rId11" xr:uid="{68F48E87-03C9-4A06-9ABC-AD2472F277D4}"/>
-    <hyperlink ref="B57" r:id="rId12" xr:uid="{4CFE8BA0-D183-4C26-9CA9-BEC5D4FEB2AF}"/>
-    <hyperlink ref="B59" r:id="rId13" xr:uid="{76008964-D3A6-4069-A099-FCBDC9806B52}"/>
-    <hyperlink ref="A13" r:id="rId14" xr:uid="{2D260EA6-B6E3-49E5-AFF7-A6AAA0D9D5F1}"/>
-    <hyperlink ref="B47" r:id="rId15" xr:uid="{BD37EAD5-5C34-4550-93BE-F5FEABEB65A8}"/>
-    <hyperlink ref="B46" r:id="rId16" xr:uid="{4E70A93A-2FD3-4A64-BFD8-40CC5D4AB6CA}"/>
-    <hyperlink ref="B48" r:id="rId17" xr:uid="{FA6B2910-1118-4545-AA35-6807A2305F66}"/>
-    <hyperlink ref="B33" r:id="rId18" xr:uid="{31F1E98B-22F1-4AAD-A4F2-1D4E1C61AC62}"/>
+    <hyperlink ref="B30" r:id="rId5" xr:uid="{20C952C0-AC93-4997-B0E6-DDB49E73E6C8}"/>
+    <hyperlink ref="B31" r:id="rId6" xr:uid="{9ED0288B-B903-4B95-A943-B00D22643BB3}"/>
+    <hyperlink ref="B50" r:id="rId7" xr:uid="{1CBDC011-B012-4D4D-85BE-815CAF394EF8}"/>
+    <hyperlink ref="B52" r:id="rId8" xr:uid="{933C97F6-B8AD-43AB-BDA5-8CE80E8B0DE0}"/>
+    <hyperlink ref="B53" r:id="rId9" xr:uid="{F9022034-5431-4C29-9A17-2E7AA4504D96}"/>
+    <hyperlink ref="B55" r:id="rId10" xr:uid="{68F48E87-03C9-4A06-9ABC-AD2472F277D4}"/>
+    <hyperlink ref="B57" r:id="rId11" xr:uid="{4CFE8BA0-D183-4C26-9CA9-BEC5D4FEB2AF}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{2D260EA6-B6E3-49E5-AFF7-A6AAA0D9D5F1}"/>
+    <hyperlink ref="B47" r:id="rId13" xr:uid="{BD37EAD5-5C34-4550-93BE-F5FEABEB65A8}"/>
+    <hyperlink ref="B46" r:id="rId14" xr:uid="{4E70A93A-2FD3-4A64-BFD8-40CC5D4AB6CA}"/>
+    <hyperlink ref="B48" r:id="rId15" xr:uid="{FA6B2910-1118-4545-AA35-6807A2305F66}"/>
+    <hyperlink ref="B33" r:id="rId16" xr:uid="{31F1E98B-22F1-4AAD-A4F2-1D4E1C61AC62}"/>
+    <hyperlink ref="B45" r:id="rId17" xr:uid="{3E511FE9-DDB3-4362-B1DB-48D4D63F2557}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>